<commit_message>
maj plans + cout alpha III
</commit_message>
<xml_diff>
--- a/Remote/Commun/dist_coûts.xlsx
+++ b/Remote/Commun/dist_coûts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\ductaironline\Remote\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A462F3FD-581A-483E-A951-07E61247D15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F08CB8-909C-4125-9DE9-DDEDCBE5D6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="6660" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="5520" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dist_coûts" sheetId="1" r:id="rId1"/>
@@ -662,7 +662,7 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +778,7 @@
         <v>25</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="D2" s="1">
         <v>45383</v>
@@ -808,7 +808,7 @@
         <v>27</v>
       </c>
       <c r="M2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N2" s="1">
         <v>45352</v>
@@ -855,7 +855,7 @@
         <v>34</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>0.67</v>
       </c>
       <c r="D3" s="1">
         <v>45383</v>
@@ -885,7 +885,7 @@
         <v>36</v>
       </c>
       <c r="M3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N3" s="1">
         <v>45352</v>
@@ -932,7 +932,7 @@
         <v>39</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>0.88</v>
       </c>
       <c r="D4" s="1">
         <v>45383</v>
@@ -1009,7 +1009,7 @@
         <v>44</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>1.8</v>
       </c>
       <c r="D5" s="1">
         <v>45383</v>
@@ -1077,7 +1077,7 @@
         <v>48</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>0.16</v>
       </c>
       <c r="D6" s="1">
         <v>45383</v>
@@ -1145,7 +1145,7 @@
         <v>52</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>0.23</v>
       </c>
       <c r="D7" s="1">
         <v>45383</v>
@@ -1207,7 +1207,7 @@
         <v>56</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>0.62</v>
       </c>
       <c r="D8" s="1">
         <v>45383</v>

</xml_diff>

<commit_message>
maj coût et users
</commit_message>
<xml_diff>
--- a/Remote/Commun/dist_coûts.xlsx
+++ b/Remote/Commun/dist_coûts.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\ductaironline\Remote\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F08CB8-909C-4125-9DE9-DDEDCBE5D6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21344B6-38E5-4D5C-8F62-919018862624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="5520" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dist_coûts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dist_coûts">dist_coûts!$A$1:$Y$25</definedName>
+    <definedName name="dist_coûts">dist_coûts!$A$1:$V$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="114">
   <si>
     <t>id</t>
   </si>
@@ -80,33 +80,21 @@
     <t>Date_Mo</t>
   </si>
   <si>
-    <t>plage_devis</t>
-  </si>
-  <si>
     <t>Date PEP Alu</t>
   </si>
   <si>
-    <t>PEP Galva</t>
-  </si>
-  <si>
     <t>€ PEP Galva</t>
   </si>
   <si>
     <t>Date PEP Galva</t>
   </si>
   <si>
-    <t>PEP Inox</t>
-  </si>
-  <si>
     <t>€ PEP Inox</t>
   </si>
   <si>
     <t>Date PEP Inox</t>
   </si>
   <si>
-    <t>PEP Alu</t>
-  </si>
-  <si>
     <t>€ PEP Alu</t>
   </si>
   <si>
@@ -137,9 +125,6 @@
     <t>4</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Coût Profil 20</t>
   </si>
   <si>
@@ -266,9 +251,6 @@
     <t>80,91</t>
   </si>
   <si>
-    <t>22/09/202422/09/2024</t>
-  </si>
-  <si>
     <t>710</t>
   </si>
   <si>
@@ -315,16 +297,103 @@
   </si>
   <si>
     <t>Griffes</t>
+  </si>
+  <si>
+    <t>Ø PEP Galva</t>
+  </si>
+  <si>
+    <t>99/99/99</t>
+  </si>
+  <si>
+    <t>99/99/100</t>
+  </si>
+  <si>
+    <t>99/99/101</t>
+  </si>
+  <si>
+    <t>99/99/102</t>
+  </si>
+  <si>
+    <t>99/99/103</t>
+  </si>
+  <si>
+    <t>99/99/104</t>
+  </si>
+  <si>
+    <t>99/99/105</t>
+  </si>
+  <si>
+    <t>99/99/106</t>
+  </si>
+  <si>
+    <t>99/99/107</t>
+  </si>
+  <si>
+    <t>99/99/108</t>
+  </si>
+  <si>
+    <t>99/99/109</t>
+  </si>
+  <si>
+    <t>99/99/110</t>
+  </si>
+  <si>
+    <t>99/99/111</t>
+  </si>
+  <si>
+    <t>99/99/112</t>
+  </si>
+  <si>
+    <t>99/99/113</t>
+  </si>
+  <si>
+    <t>99/99/114</t>
+  </si>
+  <si>
+    <t>99/99/115</t>
+  </si>
+  <si>
+    <t>Remises Utilisateur</t>
+  </si>
+  <si>
+    <t>Remises Fournisseurs</t>
+  </si>
+  <si>
+    <t>Prix Tarif</t>
+  </si>
+  <si>
+    <t>Marge</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>Actif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avertissement </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -659,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,19 +750,16 @@
     <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -737,7 +803,7 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="P1" t="s">
         <v>15</v>
@@ -755,27 +821,24 @@
         <v>19</v>
       </c>
       <c r="U1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
       <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>1.8</v>
@@ -796,7 +859,7 @@
         <v>45352</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="J2">
         <v>6.88</v>
@@ -805,7 +868,7 @@
         <v>45352</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="M2">
         <v>30</v>
@@ -813,46 +876,52 @@
       <c r="N2" s="1">
         <v>45352</v>
       </c>
-      <c r="O2">
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2">
+        <v>999</v>
+      </c>
+      <c r="U2" t="s">
+        <v>88</v>
+      </c>
+      <c r="V2">
+        <v>45</v>
+      </c>
+      <c r="W2">
         <v>500</v>
       </c>
-      <c r="P2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="X2">
+        <v>45</v>
+      </c>
+      <c r="Y2">
+        <v>50</v>
+      </c>
+      <c r="Z2">
+        <v>30</v>
+      </c>
+      <c r="AA2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
-      </c>
-      <c r="R2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V2" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" t="s">
-        <v>29</v>
-      </c>
-      <c r="X2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
       </c>
       <c r="C3">
         <v>0.67</v>
@@ -873,7 +942,7 @@
         <v>45352</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J3">
         <v>3</v>
@@ -882,7 +951,7 @@
         <v>45352</v>
       </c>
       <c r="L3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M3">
         <v>30</v>
@@ -890,46 +959,52 @@
       <c r="N3" s="1">
         <v>45352</v>
       </c>
-      <c r="O3">
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3">
+        <v>999</v>
+      </c>
+      <c r="U3" t="s">
+        <v>89</v>
+      </c>
+      <c r="V3">
+        <v>40</v>
+      </c>
+      <c r="W3">
         <v>1000</v>
       </c>
-      <c r="P3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U3" t="s">
-        <v>32</v>
-      </c>
-      <c r="V3" t="s">
-        <v>28</v>
-      </c>
-      <c r="W3" t="s">
-        <v>37</v>
-      </c>
-      <c r="X3" t="s">
-        <v>33</v>
+      <c r="X3">
+        <v>40</v>
       </c>
       <c r="Y3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="Z3">
+        <v>35</v>
+      </c>
+      <c r="AA3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C4">
         <v>0.88</v>
@@ -950,7 +1025,7 @@
         <v>45352</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J4">
         <v>0.63</v>
@@ -959,7 +1034,7 @@
         <v>45352</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M4">
         <v>10</v>
@@ -967,46 +1042,52 @@
       <c r="N4" s="1">
         <v>45352</v>
       </c>
-      <c r="O4">
+      <c r="O4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4">
+        <v>999</v>
+      </c>
+      <c r="U4" t="s">
+        <v>90</v>
+      </c>
+      <c r="V4">
+        <v>35</v>
+      </c>
+      <c r="W4">
         <v>2000</v>
       </c>
-      <c r="P4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>42</v>
-      </c>
-      <c r="R4" t="s">
-        <v>43</v>
-      </c>
-      <c r="S4" t="s">
-        <v>31</v>
-      </c>
-      <c r="T4" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4" t="s">
-        <v>32</v>
-      </c>
-      <c r="V4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W4" t="s">
-        <v>42</v>
-      </c>
-      <c r="X4" t="s">
-        <v>33</v>
+      <c r="X4">
+        <v>35</v>
       </c>
       <c r="Y4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="Z4">
+        <v>40</v>
+      </c>
+      <c r="AA4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>1.8</v>
@@ -1027,7 +1108,7 @@
         <v>45352</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J5">
         <v>9</v>
@@ -1035,46 +1116,52 @@
       <c r="K5" s="1">
         <v>45352</v>
       </c>
-      <c r="O5">
+      <c r="O5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5">
+        <v>999</v>
+      </c>
+      <c r="U5" t="s">
+        <v>91</v>
+      </c>
+      <c r="V5">
+        <v>30</v>
+      </c>
+      <c r="W5">
         <v>5000</v>
       </c>
-      <c r="P5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>46</v>
-      </c>
-      <c r="R5" t="s">
-        <v>47</v>
-      </c>
-      <c r="S5" t="s">
-        <v>31</v>
-      </c>
-      <c r="T5" t="s">
-        <v>46</v>
-      </c>
-      <c r="U5" t="s">
-        <v>32</v>
-      </c>
-      <c r="V5" t="s">
-        <v>28</v>
-      </c>
-      <c r="W5" t="s">
-        <v>46</v>
-      </c>
-      <c r="X5" t="s">
-        <v>33</v>
+      <c r="X5">
+        <v>30</v>
       </c>
       <c r="Y5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="Z5">
+        <v>45</v>
+      </c>
+      <c r="AA5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>0.16</v>
@@ -1095,7 +1182,7 @@
         <v>45352</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="J6">
         <v>11.48</v>
@@ -1103,46 +1190,52 @@
       <c r="K6" s="1">
         <v>45352</v>
       </c>
-      <c r="O6">
+      <c r="O6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6">
+        <v>999</v>
+      </c>
+      <c r="U6" t="s">
+        <v>92</v>
+      </c>
+      <c r="V6">
+        <v>25</v>
+      </c>
+      <c r="W6">
         <v>10000</v>
       </c>
-      <c r="P6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="X6">
+        <v>25</v>
+      </c>
+      <c r="Y6">
+        <v>70</v>
+      </c>
+      <c r="Z6">
         <v>50</v>
       </c>
-      <c r="R6" t="s">
-        <v>51</v>
-      </c>
-      <c r="S6" t="s">
-        <v>31</v>
-      </c>
-      <c r="T6" t="s">
-        <v>50</v>
-      </c>
-      <c r="U6" t="s">
-        <v>32</v>
-      </c>
-      <c r="V6" t="s">
-        <v>28</v>
-      </c>
-      <c r="W6" t="s">
-        <v>50</v>
-      </c>
-      <c r="X6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>0.23</v>
@@ -1163,7 +1256,7 @@
         <v>45352</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J7">
         <v>19.100000000000001</v>
@@ -1171,40 +1264,49 @@
       <c r="K7" s="1">
         <v>45352</v>
       </c>
+      <c r="O7" t="s">
+        <v>49</v>
+      </c>
       <c r="P7" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>27</v>
+      </c>
+      <c r="R7" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" t="s">
-        <v>54</v>
-      </c>
-      <c r="R7" t="s">
-        <v>55</v>
-      </c>
       <c r="S7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T7" t="s">
-        <v>54</v>
+        <v>24</v>
+      </c>
+      <c r="T7">
+        <v>999</v>
       </c>
       <c r="U7" t="s">
-        <v>32</v>
-      </c>
-      <c r="V7" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="W7" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="X7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>0.62</v>
@@ -1225,7 +1327,7 @@
         <v>45352</v>
       </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J8">
         <v>0.71</v>
@@ -1233,40 +1335,46 @@
       <c r="K8" s="1">
         <v>45352</v>
       </c>
+      <c r="O8" t="s">
+        <v>53</v>
+      </c>
       <c r="P8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R8" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" t="s">
-        <v>58</v>
-      </c>
-      <c r="R8" t="s">
-        <v>59</v>
-      </c>
       <c r="S8" t="s">
-        <v>31</v>
-      </c>
-      <c r="T8" t="s">
-        <v>58</v>
+        <v>24</v>
+      </c>
+      <c r="T8">
+        <v>999</v>
       </c>
       <c r="U8" t="s">
-        <v>32</v>
-      </c>
-      <c r="V8" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="W8" t="s">
-        <v>58</v>
-      </c>
-      <c r="X8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>1.72</v>
@@ -1287,7 +1395,7 @@
         <v>45352</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J9">
         <v>0.75</v>
@@ -1295,40 +1403,40 @@
       <c r="K9" s="1">
         <v>45352</v>
       </c>
+      <c r="O9" t="s">
+        <v>57</v>
+      </c>
       <c r="P9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>27</v>
+      </c>
+      <c r="R9" t="s">
         <v>28</v>
       </c>
-      <c r="Q9" t="s">
-        <v>62</v>
-      </c>
-      <c r="R9" t="s">
-        <v>63</v>
-      </c>
       <c r="S9" t="s">
-        <v>31</v>
-      </c>
-      <c r="T9" t="s">
-        <v>62</v>
+        <v>24</v>
+      </c>
+      <c r="T9">
+        <v>999</v>
       </c>
       <c r="U9" t="s">
-        <v>32</v>
-      </c>
-      <c r="V9" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="W9" t="s">
-        <v>62</v>
-      </c>
-      <c r="X9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -1348,40 +1456,34 @@
       <c r="H10" s="1">
         <v>45352</v>
       </c>
+      <c r="O10" t="s">
+        <v>60</v>
+      </c>
       <c r="P10" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>27</v>
+      </c>
+      <c r="R10" t="s">
         <v>28</v>
       </c>
-      <c r="Q10" t="s">
-        <v>65</v>
-      </c>
-      <c r="R10" t="s">
-        <v>66</v>
-      </c>
       <c r="S10" t="s">
-        <v>31</v>
-      </c>
-      <c r="T10" t="s">
-        <v>65</v>
+        <v>24</v>
+      </c>
+      <c r="T10">
+        <v>999</v>
       </c>
       <c r="U10" t="s">
-        <v>32</v>
-      </c>
-      <c r="V10" t="s">
-        <v>28</v>
-      </c>
-      <c r="W10" t="s">
-        <v>65</v>
-      </c>
-      <c r="X10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C11">
         <v>10.8</v>
@@ -1401,40 +1503,34 @@
       <c r="H11" s="1">
         <v>45352</v>
       </c>
+      <c r="O11" t="s">
+        <v>63</v>
+      </c>
       <c r="P11" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" t="s">
-        <v>68</v>
-      </c>
-      <c r="R11" t="s">
-        <v>69</v>
-      </c>
       <c r="S11" t="s">
-        <v>31</v>
-      </c>
-      <c r="T11" t="s">
-        <v>68</v>
+        <v>24</v>
+      </c>
+      <c r="T11">
+        <v>999</v>
       </c>
       <c r="U11" t="s">
-        <v>32</v>
-      </c>
-      <c r="V11" t="s">
-        <v>28</v>
-      </c>
-      <c r="W11" t="s">
-        <v>68</v>
-      </c>
-      <c r="X11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1454,40 +1550,34 @@
       <c r="H12" s="1">
         <v>45352</v>
       </c>
+      <c r="O12" t="s">
+        <v>65</v>
+      </c>
       <c r="P12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R12" t="s">
         <v>28</v>
       </c>
-      <c r="Q12" t="s">
-        <v>70</v>
-      </c>
-      <c r="R12" t="s">
-        <v>71</v>
-      </c>
       <c r="S12" t="s">
-        <v>31</v>
-      </c>
-      <c r="T12" t="s">
-        <v>70</v>
+        <v>24</v>
+      </c>
+      <c r="T12">
+        <v>999</v>
       </c>
       <c r="U12" t="s">
-        <v>32</v>
-      </c>
-      <c r="V12" t="s">
-        <v>28</v>
-      </c>
-      <c r="W12" t="s">
-        <v>70</v>
-      </c>
-      <c r="X12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1507,40 +1597,34 @@
       <c r="H13" s="1">
         <v>45352</v>
       </c>
+      <c r="O13" t="s">
+        <v>67</v>
+      </c>
       <c r="P13" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>27</v>
+      </c>
+      <c r="R13" t="s">
         <v>28</v>
       </c>
-      <c r="Q13" t="s">
-        <v>72</v>
-      </c>
-      <c r="R13" t="s">
-        <v>73</v>
-      </c>
       <c r="S13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T13" t="s">
-        <v>72</v>
+        <v>24</v>
+      </c>
+      <c r="T13">
+        <v>999</v>
       </c>
       <c r="U13" t="s">
-        <v>32</v>
-      </c>
-      <c r="V13" t="s">
-        <v>28</v>
-      </c>
-      <c r="W13" t="s">
-        <v>72</v>
-      </c>
-      <c r="X13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1560,40 +1644,34 @@
       <c r="H14" s="1">
         <v>45352</v>
       </c>
+      <c r="O14" t="s">
+        <v>69</v>
+      </c>
       <c r="P14" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14" t="s">
         <v>28</v>
       </c>
-      <c r="Q14" t="s">
-        <v>74</v>
-      </c>
-      <c r="R14" t="s">
-        <v>75</v>
-      </c>
       <c r="S14" t="s">
-        <v>31</v>
-      </c>
-      <c r="T14" t="s">
-        <v>74</v>
+        <v>24</v>
+      </c>
+      <c r="T14">
+        <v>999</v>
       </c>
       <c r="U14" t="s">
-        <v>32</v>
-      </c>
-      <c r="V14" t="s">
-        <v>28</v>
-      </c>
-      <c r="W14" t="s">
-        <v>74</v>
-      </c>
-      <c r="X14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1613,40 +1691,34 @@
       <c r="H15" s="1">
         <v>45352</v>
       </c>
+      <c r="O15" t="s">
+        <v>71</v>
+      </c>
       <c r="P15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="Q15" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="R15" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="S15" t="s">
-        <v>31</v>
-      </c>
-      <c r="T15" t="s">
-        <v>77</v>
+        <v>24</v>
+      </c>
+      <c r="T15">
+        <v>999</v>
       </c>
       <c r="U15" t="s">
-        <v>32</v>
-      </c>
-      <c r="V15" t="s">
-        <v>28</v>
-      </c>
-      <c r="W15" t="s">
-        <v>77</v>
-      </c>
-      <c r="X15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1666,40 +1738,34 @@
       <c r="H16" s="1">
         <v>45352</v>
       </c>
+      <c r="O16" t="s">
+        <v>73</v>
+      </c>
       <c r="P16" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>27</v>
+      </c>
+      <c r="R16" t="s">
         <v>28</v>
       </c>
-      <c r="Q16" t="s">
-        <v>79</v>
-      </c>
-      <c r="R16" t="s">
-        <v>80</v>
-      </c>
       <c r="S16" t="s">
-        <v>31</v>
-      </c>
-      <c r="T16" t="s">
-        <v>79</v>
+        <v>24</v>
+      </c>
+      <c r="T16">
+        <v>999</v>
       </c>
       <c r="U16" t="s">
-        <v>32</v>
-      </c>
-      <c r="V16" t="s">
-        <v>28</v>
-      </c>
-      <c r="W16" t="s">
-        <v>79</v>
-      </c>
-      <c r="X16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1719,40 +1785,34 @@
       <c r="H17" s="1">
         <v>45352</v>
       </c>
+      <c r="O17" t="s">
+        <v>75</v>
+      </c>
       <c r="P17" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>27</v>
+      </c>
+      <c r="R17" t="s">
         <v>28</v>
       </c>
-      <c r="Q17" t="s">
-        <v>81</v>
-      </c>
-      <c r="R17" t="s">
-        <v>82</v>
-      </c>
       <c r="S17" t="s">
-        <v>31</v>
-      </c>
-      <c r="T17" t="s">
-        <v>81</v>
+        <v>24</v>
+      </c>
+      <c r="T17">
+        <v>999</v>
       </c>
       <c r="U17" t="s">
-        <v>32</v>
-      </c>
-      <c r="V17" t="s">
-        <v>28</v>
-      </c>
-      <c r="W17" t="s">
-        <v>81</v>
-      </c>
-      <c r="X17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C18">
         <v>28.94</v>
@@ -1772,40 +1832,34 @@
       <c r="H18" s="1">
         <v>45352</v>
       </c>
+      <c r="O18" t="s">
+        <v>78</v>
+      </c>
       <c r="P18" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>27</v>
+      </c>
+      <c r="R18" t="s">
         <v>28</v>
       </c>
-      <c r="Q18" t="s">
-        <v>84</v>
-      </c>
-      <c r="R18" t="s">
-        <v>85</v>
-      </c>
       <c r="S18" t="s">
-        <v>31</v>
-      </c>
-      <c r="T18" t="s">
-        <v>84</v>
+        <v>24</v>
+      </c>
+      <c r="T18">
+        <v>999</v>
       </c>
       <c r="U18" t="s">
-        <v>32</v>
-      </c>
-      <c r="V18" t="s">
-        <v>28</v>
-      </c>
-      <c r="W18" t="s">
-        <v>84</v>
-      </c>
-      <c r="X18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C19">
         <v>43.54</v>
@@ -1826,12 +1880,12 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C20">
         <v>11.06</v>
@@ -1852,12 +1906,12 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C21">
         <v>21.12</v>
@@ -1878,12 +1932,12 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C22">
         <v>28.94</v>
@@ -1904,12 +1958,12 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C23">
         <v>36.200000000000003</v>
@@ -1930,12 +1984,12 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C24">
         <v>35.24</v>
@@ -1956,12 +2010,12 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C25">
         <v>0.94</v>
@@ -1983,6 +2037,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mise a jour pep
</commit_message>
<xml_diff>
--- a/Remote/Commun/dist_coûts.xlsx
+++ b/Remote/Commun/dist_coûts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\Remote\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625E9977-0969-4BE8-836E-9EEFB77E50CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DAA58F-666C-4CB6-B719-6BCB11BB8D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,12 +356,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,7 +670,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+      <selection activeCell="P2" sqref="P2:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,7 +824,7 @@
       <c r="O2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="3" t="s">
         <v>75</v>
       </c>
       <c r="Q2" s="2">
@@ -903,7 +904,7 @@
       <c r="O3" t="s">
         <v>27</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="3" t="s">
         <v>76</v>
       </c>
       <c r="Q3" s="2">
@@ -983,7 +984,7 @@
       <c r="O4" t="s">
         <v>31</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="3" t="s">
         <v>77</v>
       </c>
       <c r="Q4" s="2">
@@ -1054,7 +1055,7 @@
       <c r="O5" t="s">
         <v>34</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="3" t="s">
         <v>78</v>
       </c>
       <c r="Q5" s="2">
@@ -1125,7 +1126,7 @@
       <c r="O6" t="s">
         <v>37</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="3" t="s">
         <v>79</v>
       </c>
       <c r="Q6" s="2">
@@ -1196,7 +1197,7 @@
       <c r="O7" t="s">
         <v>40</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="3" t="s">
         <v>80</v>
       </c>
       <c r="Q7" s="2">
@@ -1264,7 +1265,7 @@
       <c r="O8" t="s">
         <v>43</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="3" t="s">
         <v>81</v>
       </c>
       <c r="Q8" s="2">
@@ -1332,7 +1333,7 @@
       <c r="O9" t="s">
         <v>46</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="3" t="s">
         <v>82</v>
       </c>
       <c r="Q9" s="2">
@@ -1385,7 +1386,7 @@
       <c r="O10" t="s">
         <v>48</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="3" t="s">
         <v>83</v>
       </c>
       <c r="Q10" s="2">
@@ -1444,7 +1445,7 @@
       <c r="O11" t="s">
         <v>50</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="3" t="s">
         <v>84</v>
       </c>
       <c r="Q11" s="2">
@@ -1491,7 +1492,7 @@
       <c r="O12" t="s">
         <v>51</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="3" t="s">
         <v>85</v>
       </c>
       <c r="Q12" s="2">
@@ -1538,7 +1539,7 @@
       <c r="O13" t="s">
         <v>52</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="3" t="s">
         <v>86</v>
       </c>
       <c r="Q13" s="2">
@@ -1585,7 +1586,7 @@
       <c r="O14" t="s">
         <v>53</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="3" t="s">
         <v>87</v>
       </c>
       <c r="Q14" s="2">
@@ -1632,7 +1633,7 @@
       <c r="O15" t="s">
         <v>54</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="3" t="s">
         <v>88</v>
       </c>
       <c r="Q15" s="2">
@@ -1679,7 +1680,7 @@
       <c r="O16" t="s">
         <v>55</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="3" t="s">
         <v>89</v>
       </c>
       <c r="Q16" s="2">
@@ -1726,7 +1727,7 @@
       <c r="O17" t="s">
         <v>56</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="3" t="s">
         <v>90</v>
       </c>
       <c r="Q17" s="2">
@@ -1773,7 +1774,7 @@
       <c r="O18" t="s">
         <v>58</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="3" t="s">
         <v>91</v>
       </c>
       <c r="Q18" s="2">

</xml_diff>

<commit_message>
mise a jour coûts et apropos
</commit_message>
<xml_diff>
--- a/Remote/Commun/dist_coûts.xlsx
+++ b/Remote/Commun/dist_coûts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\Remote\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DAA58F-666C-4CB6-B719-6BCB11BB8D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5911FFB8-50D7-4C3C-B3E5-8D6CCC6B3239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
   <si>
     <t>id</t>
   </si>
@@ -261,57 +261,6 @@
   </si>
   <si>
     <t>Prix tarif</t>
-  </si>
-  <si>
-    <t>14.1</t>
-  </si>
-  <si>
-    <t>12.83</t>
-  </si>
-  <si>
-    <t>12.58</t>
-  </si>
-  <si>
-    <t>15.07</t>
-  </si>
-  <si>
-    <t>17.49</t>
-  </si>
-  <si>
-    <t>20.41</t>
-  </si>
-  <si>
-    <t>22.97</t>
-  </si>
-  <si>
-    <t>31.49</t>
-  </si>
-  <si>
-    <t>34.26</t>
-  </si>
-  <si>
-    <t>54.06</t>
-  </si>
-  <si>
-    <t>60.83</t>
-  </si>
-  <si>
-    <t>73.51</t>
-  </si>
-  <si>
-    <t>76.61</t>
-  </si>
-  <si>
-    <t>89.36</t>
-  </si>
-  <si>
-    <t>105.07</t>
-  </si>
-  <si>
-    <t>118.11</t>
-  </si>
-  <si>
-    <t>149.22</t>
   </si>
   <si>
     <t>Franco</t>
@@ -670,7 +619,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P18"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,8 +773,8 @@
       <c r="O2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>75</v>
+      <c r="P2" s="3">
+        <v>14.1</v>
       </c>
       <c r="Q2" s="2">
         <v>45748</v>
@@ -904,8 +853,8 @@
       <c r="O3" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>76</v>
+      <c r="P3" s="3">
+        <v>12.83</v>
       </c>
       <c r="Q3" s="2">
         <v>45748</v>
@@ -984,8 +933,8 @@
       <c r="O4" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>77</v>
+      <c r="P4" s="3">
+        <v>12.58</v>
       </c>
       <c r="Q4" s="2">
         <v>45748</v>
@@ -1055,8 +1004,8 @@
       <c r="O5" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>78</v>
+      <c r="P5" s="3">
+        <v>15.07</v>
       </c>
       <c r="Q5" s="2">
         <v>45748</v>
@@ -1126,8 +1075,8 @@
       <c r="O6" t="s">
         <v>37</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>79</v>
+      <c r="P6" s="3">
+        <v>17.489999999999998</v>
       </c>
       <c r="Q6" s="2">
         <v>45748</v>
@@ -1197,8 +1146,8 @@
       <c r="O7" t="s">
         <v>40</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>80</v>
+      <c r="P7" s="3">
+        <v>20.41</v>
       </c>
       <c r="Q7" s="2">
         <v>45748</v>
@@ -1265,8 +1214,8 @@
       <c r="O8" t="s">
         <v>43</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>81</v>
+      <c r="P8" s="3">
+        <v>22.97</v>
       </c>
       <c r="Q8" s="2">
         <v>45748</v>
@@ -1333,8 +1282,8 @@
       <c r="O9" t="s">
         <v>46</v>
       </c>
-      <c r="P9" s="3" t="s">
-        <v>82</v>
+      <c r="P9" s="3">
+        <v>31.49</v>
       </c>
       <c r="Q9" s="2">
         <v>45748</v>
@@ -1386,8 +1335,8 @@
       <c r="O10" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="3" t="s">
-        <v>83</v>
+      <c r="P10" s="3">
+        <v>34.26</v>
       </c>
       <c r="Q10" s="2">
         <v>45748</v>
@@ -1405,7 +1354,7 @@
         <v>45748</v>
       </c>
       <c r="W10" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="Y10">
         <v>2000</v>
@@ -1445,8 +1394,8 @@
       <c r="O11" t="s">
         <v>50</v>
       </c>
-      <c r="P11" s="3" t="s">
-        <v>84</v>
+      <c r="P11" s="3">
+        <v>54.06</v>
       </c>
       <c r="Q11" s="2">
         <v>45748</v>
@@ -1492,8 +1441,8 @@
       <c r="O12" t="s">
         <v>51</v>
       </c>
-      <c r="P12" s="3" t="s">
-        <v>85</v>
+      <c r="P12" s="3">
+        <v>60.83</v>
       </c>
       <c r="Q12" s="2">
         <v>45748</v>
@@ -1539,8 +1488,8 @@
       <c r="O13" t="s">
         <v>52</v>
       </c>
-      <c r="P13" s="3" t="s">
-        <v>86</v>
+      <c r="P13" s="3">
+        <v>73.510000000000005</v>
       </c>
       <c r="Q13" s="2">
         <v>45748</v>
@@ -1586,8 +1535,8 @@
       <c r="O14" t="s">
         <v>53</v>
       </c>
-      <c r="P14" s="3" t="s">
-        <v>87</v>
+      <c r="P14" s="3">
+        <v>76.61</v>
       </c>
       <c r="Q14" s="2">
         <v>45748</v>
@@ -1633,8 +1582,8 @@
       <c r="O15" t="s">
         <v>54</v>
       </c>
-      <c r="P15" s="3" t="s">
-        <v>88</v>
+      <c r="P15" s="3">
+        <v>83.96</v>
       </c>
       <c r="Q15" s="2">
         <v>45748</v>
@@ -1680,8 +1629,8 @@
       <c r="O16" t="s">
         <v>55</v>
       </c>
-      <c r="P16" s="3" t="s">
-        <v>89</v>
+      <c r="P16" s="3">
+        <v>105.07</v>
       </c>
       <c r="Q16" s="2">
         <v>45748</v>
@@ -1727,8 +1676,8 @@
       <c r="O17" t="s">
         <v>56</v>
       </c>
-      <c r="P17" s="3" t="s">
-        <v>90</v>
+      <c r="P17" s="3">
+        <v>118.11</v>
       </c>
       <c r="Q17" s="2">
         <v>45748</v>
@@ -1774,8 +1723,8 @@
       <c r="O18" t="s">
         <v>58</v>
       </c>
-      <c r="P18" s="3" t="s">
-        <v>91</v>
+      <c r="P18" s="3">
+        <v>149.22200000000001</v>
       </c>
       <c r="Q18" s="2">
         <v>45748</v>

</xml_diff>

<commit_message>
mise a jour avant diffusion
</commit_message>
<xml_diff>
--- a/Remote/Commun/dist_coûts.xlsx
+++ b/Remote/Commun/dist_coûts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\Remote\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5911FFB8-50D7-4C3C-B3E5-8D6CCC6B3239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7933603-63F2-49D0-B0DD-733012D123EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -619,7 +619,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +798,7 @@
         <v>45</v>
       </c>
       <c r="Y2">
-        <v>75</v>
+        <v>2.25</v>
       </c>
       <c r="Z2">
         <v>30</v>
@@ -878,7 +878,7 @@
         <v>40</v>
       </c>
       <c r="Y3">
-        <v>75</v>
+        <v>2.25</v>
       </c>
       <c r="Z3">
         <v>35</v>
@@ -958,7 +958,7 @@
         <v>35</v>
       </c>
       <c r="Y4">
-        <v>75</v>
+        <v>2.25</v>
       </c>
       <c r="Z4">
         <v>40</v>
@@ -1029,7 +1029,7 @@
         <v>30</v>
       </c>
       <c r="Y5">
-        <v>75</v>
+        <v>2.25</v>
       </c>
       <c r="Z5">
         <v>45</v>
@@ -1100,7 +1100,7 @@
         <v>25</v>
       </c>
       <c r="Y6">
-        <v>75</v>
+        <v>2.25</v>
       </c>
       <c r="Z6">
         <v>50</v>
@@ -1236,7 +1236,7 @@
         <v>71</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8">
         <v>0</v>
@@ -1357,13 +1357,13 @@
         <v>75</v>
       </c>
       <c r="Y10">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="Z10">
-        <v>2100</v>
+        <v>0</v>
       </c>
       <c r="AA10">
-        <v>2200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>